<commit_message>
Added Tasks to Sprint Tracking
Added tasks for sprint 1.
</commit_message>
<xml_diff>
--- a/sprint_tracking.xlsx
+++ b/sprint_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheOneAndOnly\Documents\CS5500\book-library-web-service-scrumptious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD8FB244-20B7-4142-865C-CF719A11037B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EA32D292-29FD-4035-9486-BC6FE5DDEB36}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8988" windowHeight="5652" xr2:uid="{A38F84B6-AF10-4C3A-9953-4CB2CCCF8345}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>Task</t>
   </si>
@@ -38,6 +38,33 @@
   </si>
   <si>
     <t>TimeFrame</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Sept 24 - Sept 29</t>
+  </si>
+  <si>
+    <t>Build a Skeleton Webservice and Deploy It</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Single Table DB for Books.  Fields: BookID, BookTitle, </t>
+  </si>
+  <si>
+    <t>Create API to handle basic HTTP requests to add book, remove book, query Book by ID, and Title</t>
+  </si>
+  <si>
+    <t>Create Functions to route API functions to Postgres Functions</t>
+  </si>
+  <si>
+    <t>Deploy to Heroku</t>
+  </si>
+  <si>
+    <t>Plan next sprint (Thursday)</t>
+  </si>
+  <si>
+    <t>Collect summaries and post Sprint review to group wiki (Thursday)</t>
   </si>
 </sst>
 </file>
@@ -398,21 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B6A076-9AE7-4683-992A-4F6608B06539}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -420,10 +448,97 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kate assigned to book database task
</commit_message>
<xml_diff>
--- a/sprint_tracking.xlsx
+++ b/sprint_tracking.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahzhang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineschultz/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A01C1258-97B8-D648-A9B4-8683D28D1D64}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="20940" windowHeight="13060" xr2:uid="{A38F84B6-AF10-4C3A-9953-4CB2CCCF8345}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="SprintTracking" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
   <si>
     <t>Task</t>
   </si>
@@ -67,13 +72,13 @@
     <t>Collect summaries and post Sprint review to group wiki (Thursday)</t>
   </si>
   <si>
-    <t>Sarah</t>
+    <t>Kate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B6A076-9AE7-4683-992A-4F6608B06539}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -490,9 +495,6 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -557,7 +559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DB1F84-86A4-49B3-839F-3AB75F04F0CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updating with roles for sprint 1
</commit_message>
<xml_diff>
--- a/sprint_tracking.xlsx
+++ b/sprint_tracking.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineschultz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheOneAndOnly\Documents\CS5500\book-library-web-service-scrumptious\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43560EF1-BE5B-4B08-AB2B-CAC2B90143B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SprintTracking" sheetId="1" r:id="rId1"/>
@@ -20,18 +21,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -73,12 +74,21 @@
   </si>
   <si>
     <t>Kate</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Ani</t>
+  </si>
+  <si>
+    <t>Nathan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,23 +442,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -465,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -482,7 +492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -495,8 +505,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -509,8 +522,11 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -523,8 +539,11 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -538,7 +557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -559,14 +578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated interface and routing files
Updated library_webservice interface with functions for endpoints and corresponding helper functions in db_routing.
</commit_message>
<xml_diff>
--- a/sprint_tracking.xlsx
+++ b/sprint_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheOneAndOnly\Documents\CS5500\book-library-web-service-scrumptious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B821970C-3F16-4165-BA4E-213AEBC55D1F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0FAC3B23-4BAA-4241-83B9-D3108B90A130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -110,6 +110,27 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Authentication for users</t>
+  </si>
+  <si>
+    <t>GUID to help with sensitive information</t>
+  </si>
+  <si>
+    <t>Errors - error codes</t>
+  </si>
+  <si>
+    <t>Root endpoint - root to GET all endpoint categories that the rest api supports</t>
+  </si>
+  <si>
+    <t>HEAD - issued agains any endpoint to get just the header info.</t>
+  </si>
+  <si>
+    <t>Pagination - ?page, limit results returned to prevent dos attacks.</t>
+  </si>
+  <si>
+    <t>Schema - how to develop?</t>
   </si>
 </sst>
 </file>
@@ -474,7 +495,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,9 +707,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -697,6 +720,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated  endpoint functions and db routing functions
updated  endpoint functions and db routing functions
</commit_message>
<xml_diff>
--- a/sprint_tracking.xlsx
+++ b/sprint_tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheOneAndOnly\Documents\CS5500\book-library-web-service-scrumptious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0FAC3B23-4BAA-4241-83B9-D3108B90A130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{92FBD433-C2D5-4E8A-9AE8-F5319D41C195}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Schema - how to develop?</t>
+  </si>
+  <si>
+    <t>Write Sample Test Suite</t>
+  </si>
+  <si>
+    <t>Setup codeship and pipeline</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,31 +579,30 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -610,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
         <v>25</v>
@@ -630,10 +635,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>25</v>
@@ -650,13 +655,13 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -670,10 +675,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
@@ -690,12 +695,32 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>